<commit_message>
:sparkles: Copy font and color method
</commit_message>
<xml_diff>
--- a/sample/output.xlsx
+++ b/sample/output.xlsx
@@ -159,7 +159,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="102">
+  <fonts count="157">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -517,6 +517,13 @@
       <main:charset val="134"/>
       <main:scheme val="minor"/>
     </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="FF0000"/>
+    </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
       <main:color theme="1"/>
@@ -524,50 +531,101 @@
       <main:charset val="134"/>
       <main:scheme val="minor"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:i/>
       <main:sz val="12"/>
       <main:color theme="1"/>
       <main:name val="宋体"/>
       <main:charset val="134"/>
       <main:scheme val="minor"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:b/>
       <main:sz val="12"/>
       <main:color theme="1"/>
       <main:name val="宋体"/>
       <main:charset val="134"/>
       <main:scheme val="minor"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:i/>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <b val="true"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:u/>
       <main:sz val="12"/>
       <main:color theme="1"/>
       <main:name val="宋体"/>
       <main:charset val="134"/>
       <main:scheme val="minor"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:b/>
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:u/>
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="single"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -575,19 +633,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -595,19 +674,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -615,19 +715,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -635,19 +756,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -655,19 +797,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -675,19 +838,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -695,19 +879,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -715,19 +920,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -735,19 +961,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -755,19 +1002,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -775,26 +1043,54 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -802,19 +1098,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -822,19 +1139,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -842,19 +1180,40 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
@@ -862,26 +1221,54 @@
       <main:name val="微软雅黑"/>
       <main:charset val="134"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:sz val="12"/>
-      <main:color theme="1"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+    <font>
+      <name val="微软雅黑"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="111111"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1350,169 +1737,169 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center" wrapText="1"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
     </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
     <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>